<commit_message>
I bunch of work on the occtype editor. I am about to change the occtype control's data context and wanted to submit first. There is some excel testing work in here as well.
Former-commit-id: 723e10528b3de61de6e1301ad609a8067519f341
</commit_message>
<xml_diff>
--- a/StatisticsTests/ExcelTesting/ExcelData/Triangular.xlsx
+++ b/StatisticsTests/ExcelTesting/ExcelData/Triangular.xlsx
@@ -1590,7 +1590,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="H7" s="29">
-        <x:v>43917.37986111111</x:v>
+        <x:v>43924.44027777778</x:v>
       </x:c>
       <x:c r="I7" s="6" t="s">
         <x:v>15</x:v>
@@ -1646,7 +1646,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="H11" s="29">
-        <x:v>43917.37986111111</x:v>
+        <x:v>43924.44027777778</x:v>
       </x:c>
       <x:c r="I11" s="6" t="s">
         <x:v>15</x:v>
@@ -1702,7 +1702,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="H15" s="29">
-        <x:v>43917.37986111111</x:v>
+        <x:v>43924.44097222222</x:v>
       </x:c>
       <x:c r="I15" s="6" t="s">
         <x:v>15</x:v>
@@ -1758,7 +1758,7 @@
         <x:v>14</x:v>
       </x:c>
       <x:c r="H19" s="29">
-        <x:v>43917.37986111111</x:v>
+        <x:v>43924.44027777778</x:v>
       </x:c>
       <x:c r="I19" s="6" t="s">
         <x:v>15</x:v>

</xml_diff>